<commit_message>
Backup poll projection data investigations
</commit_message>
<xml_diff>
--- a/python/Data/poll-data-vic.xlsx
+++ b/python/Data/poll-data-vic.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danny\source\repos\Polling Analyser\python\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D70E0EF-2CCA-4C72-BAC6-6C01B82D900A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55E0CF80-90C5-46C3-A321-49B874F90439}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9945" yWindow="390" windowWidth="12570" windowHeight="16365" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="540" yWindow="7050" windowWidth="14070" windowHeight="13800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -408,9 +408,9 @@
   <dimension ref="A1:S140"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="600" topLeftCell="A106" activePane="bottomLeft"/>
+      <pane ySplit="600" activePane="bottomLeft"/>
       <selection activeCell="H1" sqref="H1:H1048576"/>
-      <selection pane="bottomLeft" activeCell="B135" sqref="B135"/>
+      <selection pane="bottomLeft" activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1662,7 +1662,7 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
-        <v>40479</v>
+        <v>40493</v>
       </c>
       <c r="B48" t="s">
         <v>12</v>
@@ -1714,7 +1714,7 @@
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
-        <v>40506</v>
+        <v>40503</v>
       </c>
       <c r="B50" t="s">
         <v>16</v>
@@ -1740,7 +1740,7 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
-        <v>40507</v>
+        <v>40506</v>
       </c>
       <c r="B51" t="s">
         <v>9</v>
@@ -1766,7 +1766,7 @@
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
-        <v>40508</v>
+        <v>40505</v>
       </c>
       <c r="B52" t="s">
         <v>16</v>
@@ -1792,7 +1792,7 @@
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
-        <v>40509</v>
+        <v>40506</v>
       </c>
       <c r="B53" t="s">
         <v>12</v>
@@ -1818,7 +1818,7 @@
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
-        <v>40510</v>
+        <v>40506</v>
       </c>
       <c r="B54" t="s">
         <v>2</v>

</xml_diff>